<commit_message>
I've updated the register spreadsheet with the new registers for monitor and control of the gpio pins.  The firmware change is documented in the previous commit.
</commit_message>
<xml_diff>
--- a/cosmic_ray_scripts/snap2_control/cr_registers.xlsx
+++ b/cosmic_ray_scripts/snap2_control/cr_registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4566bfd2e2f5f505/Documents/research/LWA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jpl365prod-my.sharepoint.com/personal/kathryn_a_plant_jpl_nasa_gov/Documents/Documents/research/LWA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{361C9EEE-8C57-47C1-9A4B-D88DE4A9EC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="14_{361C9EEE-8C57-47C1-9A4B-D88DE4A9EC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AA51FEB-11DE-4E45-8294-3608FD13700A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{028AD5E7-3E96-4DE2-B0D1-9553BB825CBB}"/>
+    <workbookView xWindow="366" yWindow="366" windowWidth="16662" windowHeight="11574" xr2:uid="{028AD5E7-3E96-4DE2-B0D1-9553BB825CBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="122">
   <si>
     <t>bitwidth</t>
   </si>
@@ -355,6 +355,51 @@
   </si>
   <si>
     <t>Counts the number of triggers output by the coincidence_trigger block. These are the internally generated triggers that made it past the veto.</t>
+  </si>
+  <si>
+    <t>gpio_in_enable</t>
+  </si>
+  <si>
+    <t>gpio_out_enable</t>
+  </si>
+  <si>
+    <t>gpio_in_count_rst</t>
+  </si>
+  <si>
+    <t>gpio_out_count_rst</t>
+  </si>
+  <si>
+    <t>Value 1 enables using the gpio_in pin</t>
+  </si>
+  <si>
+    <t>Value 1 enables using the gpio_out pin</t>
+  </si>
+  <si>
+    <t>Changing the value from 0 to 1 resets the gpio in counter.</t>
+  </si>
+  <si>
+    <t>Changing the value from 0 to 1 resets the gpio out counter.</t>
+  </si>
+  <si>
+    <t>Counts the number of rising edges on the gpio in pin, even if the pin is disable from sending a signal to the rest of the firmware.</t>
+  </si>
+  <si>
+    <t>Counts the number of rising edges on the gpio out pin, even if the pin is disable from sending a signal to the rest of the firmware.</t>
+  </si>
+  <si>
+    <t>gpio_in_count</t>
+  </si>
+  <si>
+    <t>cosmic_ray_gpiocontrol</t>
+  </si>
+  <si>
+    <t>cosmic_ray_gpio_in_count</t>
+  </si>
+  <si>
+    <t>gpio_out_count</t>
+  </si>
+  <si>
+    <t>cosmic_ray_gpio_out_count</t>
   </si>
 </sst>
 </file>
@@ -419,9 +464,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -459,7 +504,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -565,7 +610,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -707,7 +752,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -715,22 +760,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{663B0E9B-1259-49B3-93EE-CE90EC2AA12E}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.41796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.15625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -753,7 +798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -776,7 +821,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -799,7 +844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -822,7 +867,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -845,7 +890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -868,7 +913,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -891,7 +936,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -914,7 +959,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -937,7 +982,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -960,7 +1005,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -983,7 +1028,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1006,7 +1051,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1029,7 +1074,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1052,7 +1097,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1075,7 +1120,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1098,7 +1143,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1121,7 +1166,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1144,7 +1189,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -1167,7 +1212,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1190,7 +1235,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1213,7 +1258,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -1236,7 +1281,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -1259,7 +1304,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -1282,7 +1327,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -1305,7 +1350,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>102</v>
       </c>
@@ -1328,7 +1373,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>84</v>
       </c>
@@ -1351,7 +1396,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -1374,7 +1419,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -1397,7 +1442,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -1420,7 +1465,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -1443,7 +1488,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -1466,7 +1511,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -1489,7 +1534,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -1512,7 +1557,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -1535,7 +1580,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -1558,7 +1603,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -1581,7 +1626,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -1604,7 +1649,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>104</v>
       </c>
@@ -1625,6 +1670,144 @@
       </c>
       <c r="G39" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>32</v>
+      </c>
+      <c r="F40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>32</v>
+      </c>
+      <c r="F41" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>32</v>
+      </c>
+      <c r="F42" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43">
+        <v>32</v>
+      </c>
+      <c r="F43" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44">
+        <v>32</v>
+      </c>
+      <c r="C44" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>32</v>
+      </c>
+      <c r="F44" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45">
+        <v>32</v>
+      </c>
+      <c r="C45" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>32</v>
+      </c>
+      <c r="F45" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>